<commit_message>
demo-fos-persistence: fund and rate persistence
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="27880" windowHeight="18000" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="7320" yWindow="6240" windowWidth="27700" windowHeight="18000" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="team" sheetId="4" r:id="rId3"/>
     <sheet name="rm_team" sheetId="2" r:id="rId4"/>
     <sheet name="rm_cust" sheetId="5" r:id="rId5"/>
+    <sheet name="actions" sheetId="6" r:id="rId6"/>
+    <sheet name="rate" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="55">
   <si>
     <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -210,6 +212,46 @@
   </si>
   <si>
     <t>rm10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rm1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TODO: action 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TODO: action 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TODO: action 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EUR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GBP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,7 +609,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3086,9 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3341,7 +3381,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3588,8 +3628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E100"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4811,7 +4851,7 @@
         <v>81</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("insert into rm_customer_map values(", A81, ",'", B81, "',", C81,");")</f>
         <v>insert into rm_customer_map values(81,'rm9',81);</v>
       </c>
     </row>
@@ -5098,6 +5138,155 @@
       <c r="E100" t="str">
         <f t="shared" si="1"/>
         <v>insert into rm_customer_map values(100,'rm10',100);</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="str">
+        <f>CONCATENATE("insert into action values(", A1, ",'", B1, "','", C1, "','", D1,"');")</f>
+        <v>insert into action values(1,'P','rm1','TODO: action 1');</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F3" si="0">CONCATENATE("insert into action values(", A2, ",'", B2, "','", C2, "','", D2,"');")</f>
+        <v>insert into action values(2,'P','rm1','TODO: action 2');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into action values(3,'P','rm1','TODO: action 3');</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("insert into rate values('",A1,"',",B1,");")</f>
+        <v>insert into rate values('JPY',0.0089);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <v>0.12759999999999999</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D5" si="0">CONCATENATE("insert into rate values('",A2,"',",B2,");")</f>
+        <v>insert into rate values('HKD',0.1276);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>1.1315999999999999</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rate values('EUR',1.1316);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>0.1434</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rate values('CNY',0.1434);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>1.2753000000000001</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rate values('GBP',1.2753);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
db schema and data patching update
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="27780" windowHeight="18000" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="5480" yWindow="8260" windowWidth="27780" windowHeight="18000" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="63">
   <si>
     <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -274,6 +274,18 @@
   </si>
   <si>
     <t>US</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -14979,7 +14991,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J20"/>
@@ -14994,11 +15006,13 @@
     <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="79.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5" customWidth="1"/>
+    <col min="12" max="12" width="79.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -15014,8 +15028,8 @@
         <v>57</v>
       </c>
       <c r="E1" t="str">
-        <f>CONCATENATE("Issue  ", A1)</f>
-        <v>Issue  1</v>
+        <f>CONCATENATE("Issuer  ", A1)</f>
+        <v>Issuer  1</v>
       </c>
       <c r="F1">
         <v>100</v>
@@ -15023,15 +15037,21 @@
       <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="J1" t="str">
-        <f>CONCATENATE("insert into share_issue values('", B1, "', '", C1, "', '", D1, "', '", E1, "', ", F1, ", '", G1, "', ", H1, ");")</f>
-        <v>insert into share_issue values('issue 1', 'Share Issue 1(HKD)', 'HK', 'Issue  1', 100, 'HKD', 1);</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B1, "', '", C1, "', '", D1, "', '", E1, "', ", F1, ", '", G1, "', ", I1, ");")</f>
+        <v>insert into share_issue values('issue 1', 'Share Issue 1(HKD)', 'HK', 'Issuer  1', 100, 'HKD', AAA);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
@@ -15048,8 +15068,8 @@
         <v>58</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E20" si="2">CONCATENATE("Issue  ", A2)</f>
-        <v>Issue  2</v>
+        <f t="shared" ref="E2:E20" si="2">CONCATENATE("Issuer  ", A2)</f>
+        <v>Issuer  2</v>
       </c>
       <c r="F2">
         <v>80</v>
@@ -15057,17 +15077,23 @@
       <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="J2" t="str">
-        <f t="shared" ref="J2:J20" si="3">CONCATENATE("insert into share_issue values('", B2, "', '", C2, "', '", D2, "', '", E2, "', ", F2, ", '", G2, "', ", H2, ");")</f>
-        <v>insert into share_issue values('issue 2', 'Share Issue 2(GBP)', 'EU', 'Issue  2', 80, 'GBP', 2);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B2, "', '", C2, "', '", D2, "', '", E2, "', ", F2, ", '", G2, "', ", I2, ");")</f>
+        <v>insert into share_issue values('issue 2', 'Share Issue 2(GBP)', 'EU', 'Issuer  2', 80, 'GBP', AAA);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A20" si="4">A2+1</f>
+        <f t="shared" ref="A3:A20" si="3">A2+1</f>
         <v>3</v>
       </c>
       <c r="B3" t="str">
@@ -15083,7 +15109,7 @@
       </c>
       <c r="E3" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  3</v>
+        <v>Issuer  3</v>
       </c>
       <c r="F3">
         <v>60</v>
@@ -15091,17 +15117,23 @@
       <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="J3" t="str">
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B3, "', '", C3, "', '", D3, "', '", E3, "', ", F3, ", '", G3, "', ", I3, ");")</f>
+        <v>insert into share_issue values('issue 3', 'Share Issue 3(USD)', 'US', 'Issuer  3', 60, 'USD', AAA);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 3', 'Share Issue 3(USD)', 'US', 'Issue  3', 60, 'USD', 3);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="B4" t="str">
@@ -15117,7 +15149,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  4</v>
+        <v>Issuer  4</v>
       </c>
       <c r="F4">
         <v>40</v>
@@ -15125,17 +15157,23 @@
       <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="J4" t="str">
+      <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B4, "', '", C4, "', '", D4, "', '", E4, "', ", F4, ", '", G4, "', ", I4, ");")</f>
+        <v>insert into share_issue values('issue 4', 'Share Issue 4(SGD)', 'SG', 'Issuer  4', 40, 'SGD', AAA);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 4', 'Share Issue 4(SGD)', 'SG', 'Issue  4', 40, 'SGD', 4);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B5" t="str">
@@ -15151,7 +15189,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  5</v>
+        <v>Issuer  5</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -15159,17 +15197,23 @@
       <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="J5" t="str">
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B5, "', '", C5, "', '", D5, "', '", E5, "', ", F5, ", '", G5, "', ", I5, ");")</f>
+        <v>insert into share_issue values('issue 5', 'Share Issue 5(HKD)', 'HK', 'Issuer  5', 20, 'HKD', AAA);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 5', 'Share Issue 5(HKD)', 'HK', 'Issue  5', 20, 'HKD', 5);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B6" t="str">
@@ -15185,7 +15229,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  6</v>
+        <v>Issuer  6</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -15193,17 +15237,23 @@
       <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="str">
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B6, "', '", C6, "', '", D6, "', '", E6, "', ", F6, ", '", G6, "', ", I6, ");")</f>
+        <v>insert into share_issue values('issue 6', 'Share Issue 6(GBP)', 'EU', 'Issuer  6', 100, 'GBP', AAA);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 6', 'Share Issue 6(GBP)', 'EU', 'Issue  6', 100, 'GBP', 1);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="B7" t="str">
@@ -15219,7 +15269,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  7</v>
+        <v>Issuer  7</v>
       </c>
       <c r="F7">
         <v>80</v>
@@ -15227,17 +15277,23 @@
       <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="J7" t="str">
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B7, "', '", C7, "', '", D7, "', '", E7, "', ", F7, ", '", G7, "', ", I7, ");")</f>
+        <v>insert into share_issue values('issue 7', 'Share Issue 7(USD)', 'US', 'Issuer  7', 80, 'USD', AAA);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 7', 'Share Issue 7(USD)', 'US', 'Issue  7', 80, 'USD', 2);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="B8" t="str">
@@ -15253,7 +15309,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  8</v>
+        <v>Issuer  8</v>
       </c>
       <c r="F8">
         <v>60</v>
@@ -15261,18 +15317,24 @@
       <c r="G8" t="s">
         <v>56</v>
       </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="J8" t="str">
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B8, "', '", C8, "', '", D8, "', '", E8, "', ", F8, ", '", G8, "', ", I8, ");")</f>
+        <v>insert into share_issue values('issue 8', 'Share Issue 8(SGD)', 'SG', 'Issuer  8', 60, 'SGD', AAA);</v>
+      </c>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 8', 'Share Issue 8(SGD)', 'SG', 'Issue  8', 60, 'SGD', 3);</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="B9" t="str">
@@ -15288,7 +15350,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  9</v>
+        <v>Issuer  9</v>
       </c>
       <c r="F9">
         <v>40</v>
@@ -15296,17 +15358,23 @@
       <c r="G9" t="s">
         <v>51</v>
       </c>
-      <c r="H9">
-        <v>4</v>
-      </c>
-      <c r="J9" t="str">
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B9, "', '", C9, "', '", D9, "', '", E9, "', ", F9, ", '", G9, "', ", I9, ");")</f>
+        <v>insert into share_issue values('issue 9', 'Share Issue 9(HKD)', 'HK', 'Issuer  9', 40, 'HKD', AAA);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 9', 'Share Issue 9(HKD)', 'HK', 'Issue  9', 40, 'HKD', 4);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="B10" t="str">
@@ -15322,7 +15390,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  10</v>
+        <v>Issuer  10</v>
       </c>
       <c r="F10">
         <v>20</v>
@@ -15330,17 +15398,23 @@
       <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="J10" t="str">
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B10, "', '", C10, "', '", D10, "', '", E10, "', ", F10, ", '", G10, "', ", I10, ");")</f>
+        <v>insert into share_issue values('issue 10', 'Share Issue 10(GBP)', 'EU', 'Issuer  10', 20, 'GBP', AAA);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 10', 'Share Issue 10(GBP)', 'EU', 'Issue  10', 20, 'GBP', 5);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="B11" t="str">
@@ -15356,7 +15430,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  11</v>
+        <v>Issuer  11</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -15364,17 +15438,23 @@
       <c r="G11" t="s">
         <v>55</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="str">
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B11, "', '", C11, "', '", D11, "', '", E11, "', ", F11, ", '", G11, "', ", I11, ");")</f>
+        <v>insert into share_issue values('issue 11', 'Share Issue 11(USD)', 'US', 'Issuer  11', 100, 'USD', AAA);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 11', 'Share Issue 11(USD)', 'US', 'Issue  11', 100, 'USD', 1);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="B12" t="str">
@@ -15390,7 +15470,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  12</v>
+        <v>Issuer  12</v>
       </c>
       <c r="F12">
         <v>80</v>
@@ -15398,17 +15478,23 @@
       <c r="G12" t="s">
         <v>56</v>
       </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="J12" t="str">
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B12, "', '", C12, "', '", D12, "', '", E12, "', ", F12, ", '", G12, "', ", I12, ");")</f>
+        <v>insert into share_issue values('issue 12', 'Share Issue 12(SGD)', 'SG', 'Issuer  12', 80, 'SGD', AAA);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 12', 'Share Issue 12(SGD)', 'SG', 'Issue  12', 80, 'SGD', 2);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="B13" t="str">
@@ -15424,7 +15510,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  13</v>
+        <v>Issuer  13</v>
       </c>
       <c r="F13">
         <v>60</v>
@@ -15432,17 +15518,23 @@
       <c r="G13" t="s">
         <v>51</v>
       </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="J13" t="str">
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B13, "', '", C13, "', '", D13, "', '", E13, "', ", F13, ", '", G13, "', ", I13, ");")</f>
+        <v>insert into share_issue values('issue 13', 'Share Issue 13(HKD)', 'HK', 'Issuer  13', 60, 'HKD', AAA);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 13', 'Share Issue 13(HKD)', 'HK', 'Issue  13', 60, 'HKD', 3);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="B14" t="str">
@@ -15458,7 +15550,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  14</v>
+        <v>Issuer  14</v>
       </c>
       <c r="F14">
         <v>40</v>
@@ -15466,17 +15558,23 @@
       <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="J14" t="str">
+      <c r="H14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B14, "', '", C14, "', '", D14, "', '", E14, "', ", F14, ", '", G14, "', ", I14, ");")</f>
+        <v>insert into share_issue values('issue 14', 'Share Issue 14(GBP)', 'EU', 'Issuer  14', 40, 'GBP', AAA);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 14', 'Share Issue 14(GBP)', 'EU', 'Issue  14', 40, 'GBP', 4);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="B15" t="str">
@@ -15492,7 +15590,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  15</v>
+        <v>Issuer  15</v>
       </c>
       <c r="F15">
         <v>20</v>
@@ -15500,17 +15598,23 @@
       <c r="G15" t="s">
         <v>55</v>
       </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="J15" t="str">
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L15" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B15, "', '", C15, "', '", D15, "', '", E15, "', ", F15, ", '", G15, "', ", I15, ");")</f>
+        <v>insert into share_issue values('issue 15', 'Share Issue 15(USD)', 'US', 'Issuer  15', 20, 'USD', AAA);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 15', 'Share Issue 15(USD)', 'US', 'Issue  15', 20, 'USD', 5);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="B16" t="str">
@@ -15526,7 +15630,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  16</v>
+        <v>Issuer  16</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -15534,17 +15638,23 @@
       <c r="G16" t="s">
         <v>56</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="J16" t="str">
+      <c r="H16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B16, "', '", C16, "', '", D16, "', '", E16, "', ", F16, ", '", G16, "', ", I16, ");")</f>
+        <v>insert into share_issue values('issue 16', 'Share Issue 16(SGD)', 'SG', 'Issuer  16', 100, 'SGD', AAA);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 16', 'Share Issue 16(SGD)', 'SG', 'Issue  16', 100, 'SGD', 1);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="B17" t="str">
@@ -15560,7 +15670,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  17</v>
+        <v>Issuer  17</v>
       </c>
       <c r="F17">
         <v>80</v>
@@ -15568,17 +15678,23 @@
       <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="J17" t="str">
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B17, "', '", C17, "', '", D17, "', '", E17, "', ", F17, ", '", G17, "', ", I17, ");")</f>
+        <v>insert into share_issue values('issue 17', 'Share Issue 17(HKD)', 'HK', 'Issuer  17', 80, 'HKD', AAA);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 17', 'Share Issue 17(HKD)', 'HK', 'Issue  17', 80, 'HKD', 2);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="B18" t="str">
@@ -15594,7 +15710,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  18</v>
+        <v>Issuer  18</v>
       </c>
       <c r="F18">
         <v>60</v>
@@ -15602,17 +15718,23 @@
       <c r="G18" t="s">
         <v>54</v>
       </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="J18" t="str">
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B18, "', '", C18, "', '", D18, "', '", E18, "', ", F18, ", '", G18, "', ", I18, ");")</f>
+        <v>insert into share_issue values('issue 18', 'Share Issue 18(GBP)', 'EU', 'Issuer  18', 60, 'GBP', AAA);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 18', 'Share Issue 18(GBP)', 'EU', 'Issue  18', 60, 'GBP', 3);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="B19" t="str">
@@ -15628,7 +15750,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  19</v>
+        <v>Issuer  19</v>
       </c>
       <c r="F19">
         <v>40</v>
@@ -15636,17 +15758,23 @@
       <c r="G19" t="s">
         <v>55</v>
       </c>
-      <c r="H19">
-        <v>4</v>
-      </c>
-      <c r="J19" t="str">
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B19, "', '", C19, "', '", D19, "', '", E19, "', ", F19, ", '", G19, "', ", I19, ");")</f>
+        <v>insert into share_issue values('issue 19', 'Share Issue 19(USD)', 'US', 'Issuer  19', 40, 'USD', AAA);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20">
         <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 19', 'Share Issue 19(USD)', 'US', 'Issue  19', 40, 'USD', 4);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="B20" t="str">
@@ -15662,7 +15790,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="2"/>
-        <v>Issue  20</v>
+        <v>Issuer  20</v>
       </c>
       <c r="F20">
         <v>20</v>
@@ -15670,12 +15798,18 @@
       <c r="G20" t="s">
         <v>56</v>
       </c>
-      <c r="H20">
-        <v>5</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>insert into share_issue values('issue 20', 'Share Issue 20(SGD)', 'SG', 'Issue  20', 20, 'SGD', 5);</v>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" t="str">
+        <f>CONCATENATE("insert into share_issue values('", B20, "', '", C20, "', '", D20, "', '", E20, "', ", F20, ", '", G20, "', ", I20, ");")</f>
+        <v>insert into share_issue values('issue 20', 'Share Issue 20(SGD)', 'SG', 'Issuer  20', 20, 'SGD', AAA);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>